<commit_message>
Updates to Requirements Spreadsheet
</commit_message>
<xml_diff>
--- a/docs/ISA 681 Project Requirements.xlsx
+++ b/docs/ISA 681 Project Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbeach/Personal/Personal/School/ISA 681 - Secure Software/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbeach/Personal/Personal/School/ISA 681 - Secure Software/Project/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D4D815-A247-7E48-937B-CA946503FED6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0718CE08-3321-F248-8F31-36A7A020C178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27980" yWindow="4440" windowWidth="28040" windowHeight="17440" xr2:uid="{AB665DF1-95A5-4643-BE52-35B2D15F9C17}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="107">
   <si>
     <r>
       <t>o</t>
@@ -1228,9 +1228,6 @@
     <t xml:space="preserve">       Authenticate all users</t>
   </si>
   <si>
-    <t xml:space="preserve">       Prevent out-of-game collusion.</t>
-  </si>
-  <si>
     <t xml:space="preserve">       When (potential) users connect to the game system server: </t>
   </si>
   <si>
@@ -1255,9 +1252,6 @@
     <t xml:space="preserve">       Game communications and current game state of active games must not be accessible to a third party during play (other than trusted admins). </t>
   </si>
   <si>
-    <t xml:space="preserve">       Client must not trusted to make critical decisions</t>
-  </si>
-  <si>
     <t>CIA</t>
   </si>
   <si>
@@ -1282,12 +1276,6 @@
     <t>Justification</t>
   </si>
   <si>
-    <t>Python throws error on overflow?</t>
-  </si>
-  <si>
-    <t>Command input verified in code?</t>
-  </si>
-  <si>
     <t>Use TLS</t>
   </si>
   <si>
@@ -1663,13 +1651,25 @@
   </si>
   <si>
     <t xml:space="preserve"> If you are directly calling an SSL/TLS library (instead of just building on a web browser and web server), demonstrate via tests that your program: </t>
+  </si>
+  <si>
+    <t>All database interaction is through the server with data processed by the server</t>
+  </si>
+  <si>
+    <t>Python throws error on overflow? Do we handle this? Should the server restart forcing the players to re-enter their games?</t>
+  </si>
+  <si>
+    <t>Data verified on delivery to server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Client must not be trusted to make critical decisions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1721,13 +1721,32 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1742,7 +1761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
@@ -1760,6 +1779,11 @@
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2074,549 +2098,722 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C035A71-ED03-284F-9182-AD523C30A3D0}">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="124.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="8"/>
+      <c r="C2" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
       <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
       <c r="C11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>86</v>
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>87</v>
+      <c r="A14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>88</v>
+      <c r="A15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="8"/>
       <c r="C16" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="1:3" ht="23" x14ac:dyDescent="0.2">
+      <c r="B17" s="8"/>
+      <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="8"/>
+      <c r="C18" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="3:3" ht="23" x14ac:dyDescent="0.2">
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="8"/>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="8"/>
+      <c r="C27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C22" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C23" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C25" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C27" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="1" t="s">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="8"/>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="8"/>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="8"/>
+      <c r="C32" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C29" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C30" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C31" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C32" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="1" t="s">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="8"/>
+      <c r="C34" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="8"/>
+      <c r="C35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="8"/>
+      <c r="C36" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="8"/>
+      <c r="C37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="8"/>
+      <c r="C38" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="8"/>
+      <c r="C39" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C34" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C35" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C38" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="8"/>
       <c r="C41" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="8"/>
       <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="8"/>
       <c r="C44" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="8"/>
       <c r="C45" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="8"/>
       <c r="C46" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="8"/>
+      <c r="C47" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="8"/>
+      <c r="C50" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="8"/>
+      <c r="C52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="23" x14ac:dyDescent="0.2">
+      <c r="B54" s="8"/>
+      <c r="C54" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B55" s="8"/>
+      <c r="C55" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C48" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" ht="23" x14ac:dyDescent="0.2">
-      <c r="C55" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C57" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B56" s="8"/>
+      <c r="C56" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B57" s="8"/>
+      <c r="C57" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B58" s="8"/>
       <c r="C58" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B59" s="8"/>
+      <c r="C59" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" s="8"/>
+      <c r="C60" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B61" s="8"/>
+      <c r="C61" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B62" s="8"/>
+      <c r="C62" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C59" s="2" t="s">
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B63" s="8"/>
+      <c r="C63" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C60" s="2" t="s">
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B64" s="8"/>
+      <c r="C64" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C61" s="2" t="s">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" s="8"/>
+      <c r="C65" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B66" s="8"/>
+      <c r="C66" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C63" s="2" t="s">
+    <row r="67" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B67" s="8"/>
+      <c r="C67" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C64" s="2" t="s">
+    <row r="68" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B68" s="8"/>
+      <c r="C68" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C65" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C67" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C68" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B69" s="8"/>
       <c r="C69" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C70" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B70" s="8"/>
+      <c r="C70" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B71" s="8"/>
+      <c r="C71" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B72" s="8"/>
       <c r="C72" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B73" s="8"/>
       <c r="C73" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C74" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B74" s="8"/>
+      <c r="C74" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B75" s="8"/>
+      <c r="C75" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B76" s="8"/>
       <c r="C76" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C77" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="3:3" ht="23" x14ac:dyDescent="0.2">
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" spans="3:3" ht="23" x14ac:dyDescent="0.2">
-      <c r="C79" s="3" t="s">
+    <row r="77" spans="2:3" ht="23" x14ac:dyDescent="0.2">
+      <c r="B77" s="8"/>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="2:3" ht="23" x14ac:dyDescent="0.2">
+      <c r="B78" s="8"/>
+      <c r="C78" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C80" s="1" t="s">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B79" s="8"/>
+      <c r="C79" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B80" s="8"/>
+      <c r="C80" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B81" s="8"/>
       <c r="C81" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B82" s="8"/>
       <c r="C82" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B83" s="8"/>
       <c r="C83" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B84" s="8"/>
       <c r="C84" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B85" s="8"/>
       <c r="C85" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B86" s="8"/>
       <c r="C86" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B87" s="8"/>
       <c r="C87" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C88" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" s="1" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B88" s="8"/>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B89" s="8"/>
+      <c r="C89" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B90" s="8"/>
+      <c r="C90" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B91" s="8"/>
       <c r="C91" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="92" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B92" s="8"/>
       <c r="C92" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B93" s="8"/>
       <c r="C93" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B94" s="8"/>
       <c r="C94" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B95" s="8"/>
       <c r="C95" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C96" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B96" s="8"/>
+      <c r="C96" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B97" s="8"/>
       <c r="C97" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B98" s="8"/>
       <c r="C98" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B99" s="8"/>
       <c r="C99" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B100" s="8"/>
       <c r="C100" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B101" s="8"/>
       <c r="C101" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B102" s="8"/>
       <c r="C102" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C103" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="3:3" ht="23" x14ac:dyDescent="0.2">
-      <c r="C105" s="3"/>
+    <row r="104" spans="2:3" ht="23" x14ac:dyDescent="0.2">
+      <c r="C104" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>